<commit_message>
Added 2 SOAP tests
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/getActorsById.xlsx
+++ b/src/main/resources/excelsheets/getActorsById.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D002AECB-7CD7-448D-B470-E14DD8A0326B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A5506A-9181-4F4C-BFC1-EF22CAA08E7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Value </t>
   </si>
   <si>
-    <t>/Envelope/Body/getActorsByIdRequest/actor_id</t>
+    <t>/Envelope/Body/getActorsByIdResponse/actor/actor_id</t>
   </si>
 </sst>
 </file>
@@ -352,12 +352,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -375,6 +375,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>